<commit_message>
updated version of python scripts and paper
</commit_message>
<xml_diff>
--- a/StateOfArt.xlsx
+++ b/StateOfArt.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="198">
   <si>
     <t xml:space="preserve">PAPER</t>
   </si>
@@ -633,6 +633,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -654,6 +655,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -810,27 +812,27 @@
   </sheetPr>
   <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C19" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I29" activeCellId="0" sqref="I29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="82.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="82.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="53.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="37.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="42.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="5.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="5.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="9.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="6.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="4.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="4.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="8.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="38.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="82.95"/>
@@ -1183,7 +1185,9 @@
       <c r="D7" s="2" t="n">
         <v>2020</v>
       </c>
-      <c r="E7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="F7" s="2" t="n">
         <v>1340</v>
       </c>
@@ -1513,6 +1517,9 @@
       </c>
       <c r="E13" s="0" t="s">
         <v>38</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>12802</v>
       </c>
       <c r="G13" s="0" t="s">
         <v>96</v>

</xml_diff>